<commit_message>
Adding folder structure and future scripts inside the data pipeline. Note that this scripts are part of future tasks and therefore no final versions.
</commit_message>
<xml_diff>
--- a/Metadata_meteorological_stations.xlsx
+++ b/Metadata_meteorological_stations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ArcgisProjekte\Temperaturinterpolation\Datenquellen\Meteorological stations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RProjekte\Hydrologie_Quelccaya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C60D58-1887-4318-941C-EE7337A11A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DAD5F6-5931-49C0-AA41-14B7ABD4BFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="3630" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32370" yWindow="-9240" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
   <si>
     <t>Latitude</t>
   </si>
@@ -48,9 +48,6 @@
     <t>QORI-KALIS</t>
   </si>
   <si>
-    <t>AYMANJA</t>
-  </si>
-  <si>
     <t>Host</t>
   </si>
   <si>
@@ -64,6 +61,63 @@
   </si>
   <si>
     <t>Height_msnm</t>
+  </si>
+  <si>
+    <t>CARABAYA</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>meteorological</t>
+  </si>
+  <si>
+    <t>hydrological</t>
+  </si>
+  <si>
+    <t>WLS_L</t>
+  </si>
+  <si>
+    <t>WLS_O</t>
+  </si>
+  <si>
+    <t>PZ01</t>
+  </si>
+  <si>
+    <t>PZ02</t>
+  </si>
+  <si>
+    <t>PZ03</t>
+  </si>
+  <si>
+    <t>PZ04</t>
+  </si>
+  <si>
+    <t>PZ05</t>
+  </si>
+  <si>
+    <t>PZ06</t>
+  </si>
+  <si>
+    <t>PZ07</t>
+  </si>
+  <si>
+    <t>PZ08</t>
+  </si>
+  <si>
+    <t>PZ09</t>
+  </si>
+  <si>
+    <t>PZ10</t>
+  </si>
+  <si>
+    <t>PZ11</t>
+  </si>
+  <si>
+    <t>PZ12</t>
+  </si>
+  <si>
+    <t>BAROM</t>
   </si>
 </sst>
 </file>
@@ -74,7 +128,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +144,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -99,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -122,11 +182,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -140,6 +211,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -480,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,9 +570,9 @@
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -507,16 +581,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -535,10 +612,13 @@
       <c r="F2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4">
         <v>-13.87278611</v>
@@ -553,10 +633,13 @@
         <v>4175</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -573,10 +656,13 @@
         <v>5157</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -593,10 +679,13 @@
         <v>4880</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -613,10 +702,269 @@
         <v>5650</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>-13.90451</v>
+      </c>
+      <c r="C7">
+        <v>-70.846639999999994</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>-13.894270000000001</v>
+      </c>
+      <c r="C8">
+        <v>-70.87773</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>-13.89372</v>
+      </c>
+      <c r="C9">
+        <v>-70.858400000000003</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>-13.89442</v>
+      </c>
+      <c r="C10">
+        <v>-70.857550000000003</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>-13.89467</v>
+      </c>
+      <c r="C11">
+        <v>-70.855729999999994</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>-13.89411</v>
+      </c>
+      <c r="C12">
+        <v>-70.854569999999995</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>-13.893050000000001</v>
+      </c>
+      <c r="C13">
+        <v>-70.854500000000002</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>-13.893129999999999</v>
+      </c>
+      <c r="C14">
+        <v>-70.855680000000007</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>-13.894119999999999</v>
+      </c>
+      <c r="C15">
+        <v>-70.856129999999993</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>-13.89329</v>
+      </c>
+      <c r="C16">
+        <v>-70.857330000000005</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>-13.89254</v>
+      </c>
+      <c r="C17">
+        <v>-70.858559999999997</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>-13.89185</v>
+      </c>
+      <c r="C18">
+        <v>-70.857879999999994</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>-13.892469999999999</v>
+      </c>
+      <c r="C19">
+        <v>-70.859620000000007</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>-13.89254</v>
+      </c>
+      <c r="C20">
+        <v>-70.857129999999998</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>-13.89268</v>
+      </c>
+      <c r="C21">
+        <v>-70.861760000000004</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>